<commit_message>
Adicionado ex. 8 da TP2 de MNIO
</commit_message>
<xml_diff>
--- a/1/2/mnio/TP/2.xlsx
+++ b/1/2/mnio/TP/2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Desktop\ei\1\2\mnio\TP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{32C2D033-27E5-457B-8FFC-8C06EF6A9CC3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4E604FC-AD23-4E3F-82BD-9BB429D5CD56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8505" yWindow="330" windowWidth="21600" windowHeight="11385" activeTab="5" xr2:uid="{DB8C0857-D2F0-4EB4-A917-23EBA56B5D1C}"/>
+    <workbookView xWindow="5445" yWindow="435" windowWidth="21600" windowHeight="11385" activeTab="6" xr2:uid="{DB8C0857-D2F0-4EB4-A917-23EBA56B5D1C}"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="5" sheetId="4" r:id="rId4"/>
     <sheet name="6" sheetId="5" r:id="rId5"/>
     <sheet name="7" sheetId="6" r:id="rId6"/>
+    <sheet name="8" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="12">
   <si>
     <t>X</t>
   </si>
@@ -73,15 +74,18 @@
   <si>
     <t>|E3(0.5)|</t>
   </si>
+  <si>
+    <t>P3(16)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="0.000"/>
-    <numFmt numFmtId="190" formatCode="0.00000000"/>
-    <numFmt numFmtId="191" formatCode="0.000000000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.00000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -206,9 +210,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -216,7 +217,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="5" applyAlignment="1">
@@ -224,12 +225,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="191" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="190" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="190" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -249,8 +250,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4"/>
-    <xf numFmtId="191" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -586,35 +590,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>3</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -627,10 +631,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>0.2</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>1.0640000000000001</v>
       </c>
       <c r="C5">
@@ -645,7 +649,7 @@
       <c r="B6" s="2">
         <v>1.125</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <f t="shared" ref="C6:C8" si="0">(B6-B5)/(A6-A5)</f>
         <v>0.60999999999999954</v>
       </c>
@@ -665,7 +669,7 @@
         <f t="shared" si="0"/>
         <v>1.0899999999999999</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <f>(C7-C6)/(A7-A5)</f>
         <v>1.6000000000000012</v>
       </c>
@@ -686,10 +690,10 @@
         <v>1.7100000000000009</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D7:D8" si="1">(C8-C7)/(A8-A6)</f>
+        <f t="shared" ref="D8" si="1">(C8-C7)/(A8-A6)</f>
         <v>2.06666666666667</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f>(D8-D7)/(A8-A5)</f>
         <v>1.1666666666666721</v>
       </c>
@@ -699,13 +703,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>5</v>
       </c>
     </row>
@@ -713,7 +717,7 @@
       <c r="A12" s="2">
         <v>0.4</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f>B5+(A12-A5)*C6+(A12-A5)*(A12-A6)*D7+(A12-A5)*(A12-A6)*(A12-A7)*E8</f>
         <v>1.2156666666666667</v>
       </c>
@@ -723,13 +727,13 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G15" s="9"/>
+      <c r="G15" s="8"/>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17" s="9"/>
+      <c r="D17" s="8"/>
     </row>
     <row r="20" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="E20" s="9"/>
+      <c r="E20" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -756,44 +760,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="16"/>
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="A2" s="15"/>
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>3</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>86</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="3">
         <v>1.552</v>
       </c>
       <c r="C4" s="2"/>
@@ -808,7 +812,7 @@
       <c r="B5" s="2">
         <v>1.548</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <f>(B5-B4)/(A5-A4)</f>
         <v>-5.4794520547945277E-4</v>
       </c>
@@ -827,7 +831,7 @@
         <f t="shared" ref="C6:C8" si="0">(B6-B5)/(A6-A5)</f>
         <v>-7.1428571428571385E-4</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <f>(C6-C5)/(A6-A4)</f>
         <v>-1.2894613085756667E-5</v>
       </c>
@@ -849,7 +853,7 @@
         <f>(C7-C6)/(A7-A5)</f>
         <v>-3.3930033930034023E-5</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <f>(D7-D6)/(A7-A4)</f>
         <v>-1.1432293937107256E-6</v>
       </c>
@@ -874,16 +878,16 @@
         <f>(D8-D7)/(A8-A5)</f>
         <v>2.1368284841338727E-6</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <f>(E8-E7)/(A8-A4)</f>
         <v>1.3666907824352492E-7</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>4</v>
       </c>
     </row>
@@ -891,16 +895,16 @@
       <c r="A12" s="2">
         <v>100</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="6">
         <f>B4+(A12-A4)*C5+(A12-A4)*(A12-A5)*D6+(A12-A4)*(A12-A5)*(A12-A6)*E7+(A12-A4)*(A12-A5)*(A12-A6)*(A12-A7)*F8</f>
         <v>1.5429392473388306</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D13" s="9"/>
+      <c r="D13" s="8"/>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.3">
-      <c r="C19" s="9"/>
+      <c r="C19" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -931,44 +935,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>3</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>4</v>
       </c>
-      <c r="G2" s="15">
+      <c r="G2" s="14">
         <v>5</v>
       </c>
-      <c r="H2" s="15">
+      <c r="H2" s="14">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -985,119 +989,119 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>1.5249999999999999</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>0.86170000000000002</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="12">
         <f>(B5-B4)/(A5-A4)</f>
         <v>-9.0688524590163924E-2</v>
       </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>3.05</v>
       </c>
       <c r="B6" s="2">
         <v>0.73850000000000005</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="13">
         <f t="shared" ref="C6:C10" si="0">(B6-B5)/(A6-A5)</f>
         <v>-8.0786885245901635E-2</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <f>(C6-C5)/(A6-A4)</f>
         <v>3.2464391292663245E-3</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>4.5750000000000002</v>
       </c>
       <c r="B7" s="2">
         <v>0.62919999999999998</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="12">
         <f t="shared" si="0"/>
         <v>-7.1672131147541007E-2</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="13">
         <f t="shared" ref="D7:D10" si="1">(C7-C6)/(A7-A5)</f>
         <v>2.9884439666756153E-3</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="12">
         <f>(D7-D6)/(A7-A4)</f>
         <v>-5.6392385265728769E-5</v>
       </c>
-      <c r="F7" s="13"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>6.1</v>
       </c>
       <c r="B8" s="2">
         <v>0.53280000000000005</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="12">
         <f t="shared" si="0"/>
         <v>-6.321311475409834E-2</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="12">
         <f t="shared" si="1"/>
         <v>2.7734479978500548E-3</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="13">
         <f t="shared" ref="E8:E10" si="2">(D8-D7)/(A8-A5)</f>
         <v>-4.6993654388100669E-5</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <f>(E8-E7)/(A8-A4)</f>
         <v>1.5407755537095246E-6</v>
       </c>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>7.625</v>
       </c>
       <c r="B9" s="2">
         <v>0.4481</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="12">
         <f t="shared" si="0"/>
         <v>-5.5540983606557397E-2</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="12">
         <f t="shared" si="1"/>
         <v>2.5154528352593257E-3</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="12">
         <f t="shared" si="2"/>
         <v>-5.6392385265733132E-5</v>
       </c>
-      <c r="F9" s="14">
+      <c r="F9" s="13">
         <f t="shared" ref="F9:F10" si="3">(E9-E8)/(A9-A5)</f>
         <v>-1.54077555371024E-6</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G9" s="10">
         <f>(F9-F8)/(A9-A4)</f>
         <v>-4.0413785015341175E-7</v>
       </c>
-      <c r="H9" s="11"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
@@ -1106,39 +1110,39 @@
       <c r="B10" s="2">
         <v>0.37409999999999999</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="12">
         <f t="shared" si="0"/>
         <v>-4.8524590163934421E-2</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="12">
         <f t="shared" si="1"/>
         <v>2.3004568664337622E-3</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="12">
         <f t="shared" si="2"/>
         <v>-4.6993654388101319E-5</v>
       </c>
-      <c r="F10" s="13">
+      <c r="F10" s="12">
         <f t="shared" si="3"/>
         <v>1.5407755537101332E-6</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="10">
         <f>(F10-F9)/(A10-A5)</f>
         <v>4.0413785015349158E-7</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="10">
         <f>(G10-G9)/(A10-A4)</f>
         <v>8.8336142110044075E-8</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="18" t="s">
+      <c r="B13" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1146,11 +1150,11 @@
       <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="16">
         <f>B5+(A14-A5)*C6+(A14-A5)*(A14-A6)*D7+(A14-A5)*(A14-A6)*(A14-A7)*E8+(A14-A5)*(A14-A6)*(A14-A7)*(A14-A8)*F9</f>
         <v>0.60108556089875653</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="9">
         <f>ABS((A14-A5)*(A14-A6)*(A14-A7)*(A14-A8)*(A14-A9))*MAX(ABS(G9),ABS(G10))</f>
         <v>3.3607009604974666E-6</v>
       </c>
@@ -1177,61 +1181,61 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>3</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>-81.090999999999994</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>-81.058000000000007</v>
       </c>
       <c r="B5">
         <v>72</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <f>(B5-B4)/(A5-A4)</f>
         <v>727.27272727301295</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>-80.817999999999998</v>
       </c>
       <c r="B6">
@@ -1241,16 +1245,16 @@
         <f>(B6-B5)/(A6-A5)</f>
         <v>99.999999999996206</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <f>(C6-C5)/(A6-A4)</f>
         <v>-2297.7022977033903</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>-80.387</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>120</v>
       </c>
       <c r="C7">
@@ -1261,20 +1265,20 @@
         <f t="shared" ref="D7:D8" si="0">(C7-C6)/(A7-A5)</f>
         <v>-66.044031659634769</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <f>(D7-D6)/(A7-A4)</f>
         <v>3169.9691279030912</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>-79.789000000000001</v>
       </c>
       <c r="B8">
         <v>144</v>
       </c>
-      <c r="C8" s="21">
-        <f t="shared" ref="C6:C8" si="1">(B8-B7)/(A8-A7)</f>
+      <c r="C8" s="20">
+        <f t="shared" ref="C8" si="1">(B8-B7)/(A8-A7)</f>
         <v>40.133779264214112</v>
       </c>
       <c r="D8">
@@ -1285,22 +1289,22 @@
         <f>(D8-D7)/(A8-A5)</f>
         <v>40.135237364343546</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>(E8-E7)/(A8-A4)</f>
         <v>-2403.8662753753961</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1308,24 +1312,24 @@
       <c r="A12" s="1">
         <v>-80</v>
       </c>
-      <c r="B12" s="19">
+      <c r="B12" s="18">
         <f>B4+(A12-A4)*C5+(A12-A4)*(A12-A5)*D6+(A12-A4)*(A12-A5)*(A12-A6)*E7+(A12-A4)*(A12-A5)*(A12-A6)*(A12-A7)*F8</f>
         <v>303.96513048737779</v>
       </c>
       <c r="D12" s="1">
         <v>-80</v>
       </c>
-      <c r="E12" s="20">
+      <c r="E12" s="19">
         <f>B7+(A12-A7)*C8</f>
         <v>135.53177257525087</v>
       </c>
     </row>
     <row r="17" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F17" s="9"/>
-      <c r="H17" s="9"/>
+      <c r="F17" s="8"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="22" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F22" s="9"/>
+      <c r="F22" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1349,99 +1353,99 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
-        <v>0</v>
-      </c>
-      <c r="B4" s="5">
+      <c r="A4" s="4">
+        <v>0</v>
+      </c>
+      <c r="B4" s="4">
         <v>1.5708</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>0.2</v>
       </c>
       <c r="B5">
         <v>1.6596200000000001</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <f>(B5-B4)/(A5-A4)</f>
         <v>0.44410000000000061</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>0.4</v>
       </c>
       <c r="B6">
         <v>1.77752</v>
       </c>
-      <c r="C6" s="12">
+      <c r="C6" s="11">
         <f t="shared" ref="C6:C7" si="0">(B6-B5)/(A6-A5)</f>
         <v>0.58949999999999947</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D6" s="21">
         <f>(C6-C5)/(A6-A4)</f>
         <v>0.36349999999999716</v>
       </c>
-      <c r="E6" s="12"/>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="5">
+      <c r="A7" s="4">
         <v>0.6</v>
       </c>
       <c r="B7">
         <v>1.94957</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="11">
         <f t="shared" si="0"/>
         <v>0.8602500000000004</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <f>(C7-C6)/(A7-A5)</f>
         <v>0.67687500000000245</v>
       </c>
-      <c r="E7" s="22">
+      <c r="E7" s="21">
         <f>(D7-D6)/(A7-A4)</f>
         <v>0.52229166666667548</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="18" t="s">
+      <c r="B9" s="17" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1449,13 +1453,13 @@
       <c r="A10" s="1">
         <v>0.3</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B10" s="19">
         <f>B4+(A10-A4)*C5+(A10-A4)*(A10-A5)*D6+(A10-A4)*(A10-A5)*(A10-A6)*E7</f>
         <v>1.7133681250000001</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H13" s="9"/>
+      <c r="H13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1470,8 +1474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B94EC30E-3120-4336-9FEA-E66EA0B56787}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1480,39 +1484,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
     </row>
     <row r="2" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="15">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15">
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
         <v>1</v>
       </c>
-      <c r="D2" s="15">
+      <c r="D2" s="14">
         <v>2</v>
       </c>
-      <c r="E2" s="15">
+      <c r="E2" s="14">
         <v>3</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="22">
         <v>4</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="22">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1525,10 +1529,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>0.2</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>0.57926</v>
       </c>
       <c r="C5">
@@ -1537,13 +1541,13 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>0.4</v>
       </c>
       <c r="B6" s="1">
         <v>0.65542</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <f t="shared" ref="C6:C9" si="0">(B6-B5)/(A6-A5)</f>
         <v>0.38080000000000003</v>
       </c>
@@ -1553,7 +1557,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>0.6</v>
       </c>
       <c r="B7" s="1">
@@ -1563,7 +1567,7 @@
         <f t="shared" si="0"/>
         <v>0.35165000000000007</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <f t="shared" ref="D7:D9" si="1">(C7-C6)/(A7-A5)</f>
         <v>-7.2874999999999884E-2</v>
       </c>
@@ -1573,7 +1577,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>0.8</v>
       </c>
       <c r="B8" s="1">
@@ -1587,7 +1591,7 @@
         <f t="shared" si="1"/>
         <v>-9.9250000000001143E-2</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <f t="shared" ref="E8:E9" si="2">(D8-D7)/(A8-A5)</f>
         <v>-4.3958333333335424E-2</v>
       </c>
@@ -1625,13 +1629,13 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1639,17 +1643,211 @@
       <c r="A12" s="1">
         <v>0.5</v>
       </c>
-      <c r="B12" s="20">
+      <c r="B12" s="19">
         <f>B5+(A12-A5)*C6+(A12-A5)*(A12-A6)*D7+(A12-A5)*(A12-A6)*(A12-A7)*E8</f>
         <v>0.69144562500000006</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="9">
         <f>ABS((A12-A5)*(A12-A6)*(A12-A7)*(A12-A8))*ABS(MAX(F8:F9))</f>
         <v>2.0156250000007131E-5</v>
       </c>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.3">
-      <c r="F20" s="9"/>
+      <c r="F20" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6837DD4A-1A9C-410D-A5AE-7DF2A9679865}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="7" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B1" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+    </row>
+    <row r="2" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="14">
+        <v>0</v>
+      </c>
+      <c r="C2" s="14">
+        <v>1</v>
+      </c>
+      <c r="D2" s="14">
+        <v>2</v>
+      </c>
+      <c r="E2" s="14">
+        <v>3</v>
+      </c>
+      <c r="F2" s="22">
+        <v>4</v>
+      </c>
+      <c r="G2" s="22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>10</v>
+      </c>
+      <c r="B5" s="4">
+        <v>227.04</v>
+      </c>
+      <c r="C5">
+        <f>(B5-B4)/(A5-A4)</f>
+        <v>22.704000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>362.78</v>
+      </c>
+      <c r="C6" s="4">
+        <f t="shared" ref="C6:C9" si="0">(B6-B5)/(A6-A5)</f>
+        <v>27.147999999999996</v>
+      </c>
+      <c r="D6">
+        <f>(C6-C5)/(A6-A4)</f>
+        <v>0.29626666666666635</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>517.35</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>30.914000000000009</v>
+      </c>
+      <c r="D7" s="4">
+        <f t="shared" ref="D7:D9" si="1">(C7-C6)/(A7-A5)</f>
+        <v>0.37660000000000127</v>
+      </c>
+      <c r="E7">
+        <f>(D7-D6)/(A7-A4)</f>
+        <v>4.0166666666667464E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>22.5</v>
+      </c>
+      <c r="B8">
+        <v>602.97</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>34.248000000000005</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.44453333333333284</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" ref="E8:E9" si="2">(D8-D7)/(A8-A5)</f>
+        <v>5.4346666666665253E-3</v>
+      </c>
+      <c r="F8">
+        <f>(E8-E7)/(A8-A4)</f>
+        <v>6.3022222222212387E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>901.67</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>39.826666666666661</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.55786666666666562</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>7.5555555555555194E-3</v>
+      </c>
+      <c r="F9">
+        <f>(E9-E8)/(A9-A5)</f>
+        <v>1.0604444444444971E-4</v>
+      </c>
+      <c r="G9">
+        <f>(F9-F8)/(A9-A4)</f>
+        <v>1.4340740740745776E-6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>16</v>
+      </c>
+      <c r="B12" s="19">
+        <f>B5+(A12-A5)*C6+(A12-A5)*(A12-A6)*D7+(A12-A5)*(A12-A6)*(A12-A7)*E8</f>
+        <v>392.05716800000005</v>
+      </c>
+      <c r="C12" s="9">
+        <f>ABS((A12-A5)*(A12-A6)*(A12-A7)*(A12-A8))*ABS(MAX(F8:F9))</f>
+        <v>1.6542933333334155E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>